<commit_message>
stykliste opdateret. Calculationsklasse opdateret (Småfejl)
</commit_message>
<xml_diff>
--- a/Materialer-Skruer-Tilbehør/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
+++ b/Materialer-Skruer-Tilbehør/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\google drive\Datamatiker\2_semester\Eksamensprojekt\Kode\Materialer-Skruer-Tilbehør\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6390C38-E1DF-492A-AE69-CD603768828F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EC4C66-7301-4ABA-B9CE-774EC2A38864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Materialetype</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>45 x 145 mm</t>
+  </si>
+  <si>
+    <t>1 m</t>
   </si>
 </sst>
 </file>
@@ -485,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -534,12 +537,12 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -553,7 +556,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -567,7 +570,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -581,7 +584,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -595,19 +598,19 @@
         <v>574</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -621,7 +624,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -635,17 +638,17 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -659,12 +662,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -678,7 +681,7 @@
         <v>74.95</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -692,7 +695,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -706,7 +709,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -720,7 +723,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
@@ -734,7 +737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
@@ -748,12 +751,12 @@
         <v>409</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
@@ -767,7 +770,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
@@ -781,12 +784,12 @@
         <v>14.76</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>37</v>
       </c>
@@ -800,7 +803,7 @@
         <v>48.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>40</v>
       </c>
@@ -814,7 +817,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
@@ -833,47 +836,53 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>47</v>
       </c>

</xml_diff>